<commit_message>
Added slides and post.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jasonbryer/Dropbox (Personal)/School/Teaching/DAV5300 2025 Spring/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbryer/Dropbox (Personal)/School/Teaching/DAV5300 2025 Spring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF1D360F-B1FD-CA4C-BDE2-C586B4F30652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE67238-D8AA-E34D-BBFE-3E9183933909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2380" yWindow="4000" windowWidth="25340" windowHeight="14540" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="67">
   <si>
     <t>Date</t>
   </si>
@@ -233,6 +233,9 @@
   </si>
   <si>
     <t>/slides/07-Inference_for_Numerical_Data.html</t>
+  </si>
+  <si>
+    <t>/slides/08-Linear_Regression.html</t>
   </si>
 </sst>
 </file>
@@ -626,7 +629,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -794,6 +797,9 @@
       </c>
       <c r="C8" t="s">
         <v>26</v>
+      </c>
+      <c r="D8" t="s">
+        <v>66</v>
       </c>
       <c r="E8" t="s">
         <v>46</v>

</xml_diff>